<commit_message>
Changed tableau de synthese
</commit_message>
<xml_diff>
--- a/assets/Tableau_de_Synthese.xlsx
+++ b/assets/Tableau_de_Synthese.xlsx
@@ -9,14 +9,14 @@
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$27</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t xml:space="preserve">AP1 : évolution dun site web (Symfony) avec qualité de code, accès avec authentification (Keycloak), tests unitaire et fonctionnels, référencement, mise en ligne du site, de la BDD et du serveur Keycloak : mise à disposition des formations  de la médiathèque Mediatek86 (code source, BDD, tests unitaires et fonctionnels, documentation technique, documentation utilisateur)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AP3 : évolution d'une application de bureau en C# avec qualité de code, accès avec authentification, tests unitaires et fonctionnels, logs, mise en ligne de la BDD, création d'un installeur : gestion des documents de la médiathèque Mediatek86 (code source, BDD, tests unitaires et fonctionnels, fichier de logs, documentation technique, documentation utilisateur)</t>
   </si>
   <si>
     <t xml:space="preserve">AP : création d'une application de bureau en C# avec qualité de code, accès avec authentification, exploitation de BDD, création d'un installeur : gestion des employés de la médiathèque Mediatek86 (code source, BDD, documentation technique, documentation utilisateur)</t>
@@ -1221,7 +1218,7 @@
       <c r="G7" s="19"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" s="13" customFormat="1" ht="42.75">
+    <row r="8" s="13" customFormat="1" ht="28.5">
       <c r="A8" s="21" t="s">
         <v>24</v>
       </c>
@@ -1277,7 +1274,7 @@
       </c>
       <c r="H10" s="24"/>
     </row>
-    <row r="11" s="13" customFormat="1" ht="85.5">
+    <row r="11" s="13" customFormat="1" ht="57">
       <c r="A11" s="21" t="s">
         <v>28</v>
       </c>
@@ -1297,113 +1294,103 @@
       </c>
       <c r="H11" s="24"/>
     </row>
-    <row r="12" s="13" customFormat="1" ht="85.5">
+    <row r="12" s="13" customFormat="1" ht="28.5">
       <c r="A12" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="22"/>
-      <c r="C12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="23"/>
       <c r="F12" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="G12" s="23"/>
       <c r="H12" s="24"/>
     </row>
-    <row r="13" s="13" customFormat="1" ht="85.5">
-      <c r="A13" s="21" t="s">
-        <v>30</v>
-      </c>
+    <row r="13" s="13" customFormat="1" ht="14.25">
+      <c r="A13" s="21"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="F13" s="23"/>
       <c r="G13" s="23"/>
       <c r="H13" s="24"/>
     </row>
-    <row r="14" s="13" customFormat="1" ht="14.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" s="13" customFormat="1" ht="16.5">
-      <c r="A15" s="25" t="s">
+    <row r="14" s="13" customFormat="1" ht="16.5">
+      <c r="A14" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" s="13" customFormat="1" ht="14.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" s="13" customFormat="1" ht="28.5">
+      <c r="A16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="27"/>
-    </row>
-    <row r="16" s="13" customFormat="1" ht="14.25">
-      <c r="A16" s="21"/>
       <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+      <c r="C16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="F16" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="H16" s="24"/>
     </row>
-    <row r="17" s="13" customFormat="1" ht="28.5">
-      <c r="A17" s="21" t="s">
+    <row r="17" s="13" customFormat="1" ht="14.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" s="13" customFormat="1" ht="16.5">
+      <c r="A18" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="24"/>
-    </row>
-    <row r="18" s="13" customFormat="1" ht="14.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="19" s="13" customFormat="1" ht="16.5">
-      <c r="A19" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="27"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
+    </row>
+    <row r="19" s="13" customFormat="1" ht="14.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
     </row>
     <row r="20" s="13" customFormat="1" ht="14.25">
       <c r="A20" s="21"/>
@@ -1466,185 +1453,41 @@
       <c r="H25" s="24"/>
     </row>
     <row r="26" s="13" customFormat="1" ht="14.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
     </row>
     <row r="27" s="13" customFormat="1" ht="14.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
-    </row>
-    <row r="28" s="13" customFormat="1" ht="14.25">
-      <c r="A28" s="32"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-    </row>
-    <row r="29" s="0" customFormat="1">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-    </row>
-    <row r="30" s="0" customFormat="1">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-    </row>
-    <row r="31" s="0" customFormat="1">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-    </row>
-    <row r="32" s="0" customFormat="1">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
-    </row>
-    <row r="33" s="0" customFormat="1">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-    </row>
-    <row r="34" s="0" customFormat="1">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-    </row>
-    <row r="35" s="0" customFormat="1">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-    </row>
-    <row r="36" s="0" customFormat="1">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-    </row>
-    <row r="37" s="0" customFormat="1">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-    </row>
-    <row r="38" s="0" customFormat="1">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-    </row>
-    <row r="39" s="0" customFormat="1">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-    </row>
-    <row r="40" s="0" customFormat="1">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-    </row>
-    <row r="41" s="0" customFormat="1">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
-    </row>
-    <row r="42" s="0" customFormat="1">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-    </row>
-    <row r="43" s="0" customFormat="1">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-    </row>
+      <c r="A27" s="32"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+    </row>
+    <row r="28" s="0" customFormat="1"/>
+    <row r="29" s="0" customFormat="1"/>
+    <row r="30" s="0" customFormat="1"/>
+    <row r="31" s="0" customFormat="1"/>
+    <row r="32" s="0" customFormat="1"/>
+    <row r="33" s="0" customFormat="1"/>
+    <row r="34" s="0" customFormat="1"/>
+    <row r="35" s="0" customFormat="1"/>
+    <row r="36" s="0" customFormat="1"/>
+    <row r="37" s="0" customFormat="1"/>
+    <row r="38" s="0" customFormat="1"/>
+    <row r="39" s="0" customFormat="1"/>
+    <row r="40" s="0" customFormat="1"/>
+    <row r="41" s="0" customFormat="1"/>
+    <row r="42" s="0" customFormat="1"/>
+    <row r="43" s="0" customFormat="1"/>
     <row r="44" s="0" customFormat="1"/>
     <row r="45" s="0" customFormat="1"/>
     <row r="46" s="0" customFormat="1"/>
@@ -1675,7 +1518,6 @@
     <row r="71" s="0" customFormat="1"/>
     <row r="72" s="0" customFormat="1"/>
     <row r="73" s="0" customFormat="1"/>
-    <row r="74" s="0" customFormat="1"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A1:F1"/>
@@ -1687,8 +1529,8 @@
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.19685039370078738" right="0.19685039370078738" top="0.19685039370078738" bottom="0.19685039370078738" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>